<commit_message>
policy working for four users
</commit_message>
<xml_diff>
--- a/docs/access_matrix.xlsx
+++ b/docs/access_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/working/permitta/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A37E8DDC-7531-4B46-92C7-4F6A0A2E150F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4682331B-B739-094E-A2A8-D9727B7AA4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-4180" windowWidth="51200" windowHeight="28300" xr2:uid="{BD5A815E-05AF-D341-A68E-715F851C6A7B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{BD5A815E-05AF-D341-A68E-715F851C6A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="41">
   <si>
     <t>Catalog</t>
   </si>
@@ -349,11 +349,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -413,6 +410,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -729,13 +732,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483F398A-BB8E-F04B-81B8-9D11DDFA2BA6}">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,42 +747,37 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="16" width="10.83203125" style="2"/>
-    <col min="17" max="20" width="8.5" style="2" customWidth="1"/>
+    <col min="5" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="17" width="6.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="20" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="20" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="1" t="s">
+      <c r="L1" s="20"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+    </row>
+    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -792,56 +790,47 @@
       <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -851,32 +840,29 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="11"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="Q3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -889,28 +875,25 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="11" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="11"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="11"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -920,32 +903,29 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="11"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="Q5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -955,36 +935,29 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T6" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -994,36 +967,29 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1033,36 +999,29 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="11"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="11"/>
+      <c r="O8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="Q8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T8" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1072,32 +1031,25 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T9" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1107,32 +1059,25 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="11"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="10"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="R10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S10" s="10"/>
-      <c r="T10" s="11"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1142,36 +1087,29 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="R11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T11" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1181,30 +1119,25 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="11"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="10"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="11"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T12" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1214,202 +1147,195 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="R13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="T13" s="14"/>
-    </row>
-    <row r="16" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="16" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="R17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="T17" s="8"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+      <c r="N17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T18" s="11"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
+      <c r="N18" s="8"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="10"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="16"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="15"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B21" s="4" t="s">
+      <c r="N20" s="8"/>
+      <c r="O20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q20" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
+      <c r="N21" s="8"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="N22" s="14"/>
+      <c r="O22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" s="4"/>
       <c r="Q22" s="15"/>
-      <c r="R22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S22" s="5"/>
-      <c r="T22" s="16"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B24" s="4" t="s">
+      <c r="N23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q24" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="11"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
+      <c r="N24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="N25" s="14"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="Q25" s="15"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="T25" s="16"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S26" s="10"/>
-      <c r="T26" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
+      <c r="N26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S27" s="10"/>
-      <c r="T27" s="11"/>
-    </row>
-    <row r="28" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="N27" s="8"/>
+      <c r="O27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="10"/>
+    </row>
+    <row r="28" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="N28" s="11"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1441,10 +1367,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="N1:Q1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rego policy now supports column masking by expression
</commit_message>
<xml_diff>
--- a/docs/access_matrix.xlsx
+++ b/docs/access_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/working/permitta/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4682331B-B739-094E-A2A8-D9727B7AA4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A57E1F-9E14-0B4A-9CB3-C1D16E1FFBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{BD5A815E-05AF-D341-A68E-715F851C6A7B}"/>
+    <workbookView xWindow="-46700" yWindow="-2660" windowWidth="30240" windowHeight="18880" xr2:uid="{BD5A815E-05AF-D341-A68E-715F851C6A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>Column</t>
   </si>
   <si>
-    <t>column2</t>
-  </si>
-  <si>
     <t>Read</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>Procedures</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -349,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -373,9 +373,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -403,6 +400,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -410,12 +413,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -738,7 +735,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,29 +750,29 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="19" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="19" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -790,44 +787,44 @@
       <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="P2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -841,16 +838,13 @@
         <v>5</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
+      <c r="J3" s="9"/>
       <c r="K3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
+      <c r="M3" s="9"/>
       <c r="N3" s="6" t="s">
         <v>23</v>
       </c>
@@ -873,25 +867,20 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
+      <c r="J4" s="9"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="10"/>
+      <c r="M4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -904,24 +893,20 @@
         <v>6</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
+      <c r="J5" s="9"/>
       <c r="K5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="10" t="s">
+      <c r="M5" s="9"/>
+      <c r="N5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -938,24 +923,21 @@
       <c r="E6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
+      <c r="J6" s="9"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="10"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -970,24 +952,21 @@
       <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="8"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="10"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="9"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1000,24 +979,20 @@
         <v>9</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="10" t="s">
+      <c r="M8" s="9"/>
+      <c r="O8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1032,20 +1007,15 @@
         <v>10</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="10"/>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="9"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10" t="s">
+      <c r="M9" s="9"/>
+      <c r="Q9" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1060,22 +1030,17 @@
         <v>12</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="10"/>
+      <c r="M10" s="9"/>
+      <c r="O10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1090,24 +1055,21 @@
       <c r="E11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q11" s="10"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1120,22 +1082,18 @@
         <v>14</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="10"/>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="9"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q12" s="10"/>
+      <c r="M12" s="9"/>
+      <c r="P12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1147,27 +1105,27 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="13"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="12"/>
     </row>
     <row r="16" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -1193,22 +1151,21 @@
         <v>18</v>
       </c>
       <c r="N18" s="8"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q18" s="10"/>
+      <c r="P18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="9"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N19" s="14" t="s">
+      <c r="N19" s="13" t="s">
         <v>23</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="15"/>
+      <c r="Q19" s="14"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1218,13 +1175,13 @@
         <v>17</v>
       </c>
       <c r="N20" s="8"/>
-      <c r="O20" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q20" s="10" t="s">
+      <c r="O20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q20" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1233,9 +1190,7 @@
         <v>18</v>
       </c>
       <c r="N21" s="8"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="10" t="s">
+      <c r="Q21" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1243,12 +1198,12 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="14"/>
+      <c r="N22" s="13"/>
       <c r="O22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="P22" s="4"/>
-      <c r="Q22" s="15"/>
+      <c r="Q22" s="14"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1260,11 +1215,10 @@
       <c r="N23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q23" s="10" t="s">
+      <c r="P23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q23" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1275,20 +1229,18 @@
       <c r="N24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="10"/>
+      <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="14"/>
+      <c r="N25" s="13"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q25" s="15"/>
+      <c r="Q25" s="14"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1300,11 +1252,10 @@
       <c r="N26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O26" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="10" t="s">
+      <c r="O26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q26" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1313,56 +1264,55 @@
         <v>18</v>
       </c>
       <c r="N27" s="8"/>
-      <c r="O27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="10"/>
+      <c r="O27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="9"/>
     </row>
     <row r="28" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N28" s="11"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="13" t="s">
+      <c r="N28" s="10"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds decision logs, minor timestamp fixes and relaignment with datalake catalog
</commit_message>
<xml_diff>
--- a/docs/access_matrix.xlsx
+++ b/docs/access_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/working/permitta/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A57E1F-9E14-0B4A-9CB3-C1D16E1FFBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78603B6-3CDD-5A42-A7BB-39AAC0C13B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46700" yWindow="-2660" windowWidth="30240" windowHeight="18880" xr2:uid="{BD5A815E-05AF-D341-A68E-715F851C6A7B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{BD5A815E-05AF-D341-A68E-715F851C6A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="42">
   <si>
     <t>Catalog</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Table</t>
   </si>
   <si>
-    <t>iceberg</t>
-  </si>
-  <si>
     <t>hr</t>
   </si>
   <si>
@@ -158,6 +155,12 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>datalake</t>
   </si>
 </sst>
 </file>
@@ -729,13 +732,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483F398A-BB8E-F04B-81B8-9D11DDFA2BA6}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,25 +753,25 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="22"/>
       <c r="H1" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" s="21"/>
       <c r="J1" s="22"/>
       <c r="K1" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L1" s="21"/>
       <c r="M1" s="22"/>
       <c r="N1" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O1" s="19"/>
       <c r="P1" s="19"/>
@@ -785,89 +788,89 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="G2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>19</v>
-      </c>
       <c r="H2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>19</v>
-      </c>
       <c r="K2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="17" t="s">
-        <v>19</v>
-      </c>
       <c r="N2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="P2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="17" t="s">
         <v>31</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
       <c r="E3" s="8"/>
       <c r="G3" s="9"/>
       <c r="H3" s="8"/>
       <c r="J3" s="9"/>
       <c r="K3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8"/>
       <c r="G4" s="9"/>
@@ -875,53 +878,53 @@
       <c r="J4" s="9"/>
       <c r="K4" s="8"/>
       <c r="M4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="8"/>
       <c r="G5" s="9"/>
       <c r="H5" s="8"/>
       <c r="J5" s="9"/>
       <c r="K5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
@@ -929,390 +932,416 @@
       <c r="K6" s="8"/>
       <c r="M6" s="9"/>
       <c r="N6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="G7" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="8"/>
       <c r="J7" s="9"/>
       <c r="K7" s="8"/>
       <c r="M7" s="9"/>
       <c r="N7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="G8" s="9"/>
-      <c r="H8" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="H8" s="8"/>
       <c r="J8" s="9"/>
       <c r="K8" s="8"/>
       <c r="M8" s="9"/>
+      <c r="N8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="O8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="8"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="1" t="s">
-        <v>23</v>
+      <c r="H9" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="8"/>
       <c r="M9" s="9"/>
+      <c r="O9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="Q9" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E10" s="8"/>
       <c r="G10" s="9"/>
       <c r="H10" s="8"/>
-      <c r="J10" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="I10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="9"/>
       <c r="K10" s="8"/>
       <c r="M10" s="9"/>
-      <c r="O10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q10" s="9"/>
+      <c r="Q10" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="E11" s="8"/>
       <c r="G11" s="9"/>
       <c r="H11" s="8"/>
-      <c r="J11" s="9"/>
+      <c r="J11" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="K11" s="8"/>
       <c r="M11" s="9"/>
-      <c r="N11" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="O11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="8"/>
       <c r="J12" s="9"/>
       <c r="K12" s="8"/>
       <c r="M12" s="9"/>
+      <c r="N12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="P12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="12"/>
-    </row>
-    <row r="16" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q17" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="8"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="8"/>
+      <c r="M13" s="9"/>
+      <c r="P13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="9"/>
+    </row>
+    <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="12"/>
+    </row>
+    <row r="17" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
       <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N18" s="8"/>
-      <c r="P18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q18" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N19" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="N19" s="8"/>
+      <c r="P19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q19" s="9"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
       <c r="B20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q20" s="9" t="s">
-        <v>23</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="14"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
       <c r="B21" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N21" s="8"/>
+      <c r="O21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="Q21" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N22" s="13"/>
-      <c r="O22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="N22" s="8"/>
+      <c r="Q22" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" s="13"/>
+      <c r="O23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="14"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q23" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="N24" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q24" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N25" s="13"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q25" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
       <c r="B26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="13"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q26" s="14"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N26" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q26" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
+      <c r="N28" s="8"/>
+      <c r="O28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" s="9"/>
+    </row>
+    <row r="29" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N27" s="8"/>
-      <c r="O27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q27" s="9"/>
-    </row>
-    <row r="28" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N28" s="10"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>33</v>
+      <c r="N29" s="10"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>34</v>
+      <c r="A32" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the model for data objects and fixed all tests
</commit_message>
<xml_diff>
--- a/docs/access_matrix.xlsx
+++ b/docs/access_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/working/permitta/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78603B6-3CDD-5A42-A7BB-39AAC0C13B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5D605D-4316-BA4D-8958-01D852A90B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{BD5A815E-05AF-D341-A68E-715F851C6A7B}"/>
   </bookViews>
@@ -154,13 +154,13 @@
     <t>Procedures</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>datalake</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
+  </si>
+  <si>
+    <t>phone</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,7 +746,7 @@
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="10.83203125" style="1"/>
     <col min="14" max="17" width="6.83203125" style="1" customWidth="1"/>
   </cols>
@@ -832,7 +832,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -870,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="8"/>
       <c r="G4" s="9"/>
@@ -887,7 +887,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -953,7 +953,7 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" s="8"/>
       <c r="G7" s="9" t="s">
@@ -970,7 +970,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -1352,5 +1352,6 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>